<commit_message>
analysis of deviation money
</commit_message>
<xml_diff>
--- a/temp/listado_metricas.xlsx
+++ b/temp/listado_metricas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo\phc\api-xm\solares-operacion\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo\phc\mercados\api-xm\solares-operacion\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF27603-A719-4138-8AC4-E6143AE1F38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4AB7CD-66E9-429F-9DE6-483DE2931968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1861,8 +1861,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D200" sqref="D200"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2142,7 +2142,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -6588,7 +6588,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -7310,7 +7310,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -8070,7 +8070,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -8786,7 +8786,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -9076,9 +9076,21 @@
   <autoFilter ref="A1:L190" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="3">
       <filters>
-        <filter val="Disponibilidad Comercial por Recurso"/>
-        <filter val="Disponibilidad Declarada por Recurso"/>
-        <filter val="Disponibilidad Real por Recurso"/>
+        <filter val="FAZNI Precio por Sistema"/>
+        <filter val="Máximo Precio de Oferta Nacional por Sistema"/>
+        <filter val="Precio Bolsa Nacional Ponderado por Sistema"/>
+        <filter val="Precio Bolsa Nacional por Sistema"/>
+        <filter val="Precio Bolsa Promedio Aritmético TX1 por Sistema"/>
+        <filter val="Precio Cargo por Confiabilidad por Recurso"/>
+        <filter val="Precio de Oferta de Despacho por Recurso"/>
+        <filter val="Precio de Oferta Ideal por Recurso"/>
+        <filter val="Precio Escasez Activación por Sistema"/>
+        <filter val="Precio Escasez Ponderado por Sistema"/>
+        <filter val="Precio Escasez por Sistema"/>
+        <filter val="Precio Marginal Escasez por Sistema"/>
+        <filter val="Precio Promedio Contrato por Sistema"/>
+        <filter val="Precio Promedio Contratos No Regulados por Sistema"/>
+        <filter val="Precio Promedio Contratos Regulados por Sistema"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>